<commit_message>
Senior and Sys Admin
</commit_message>
<xml_diff>
--- a/OU Year 3 - 2018/W19 Semester/Senior Project/Projects/Sprints/Sprint 2/Efforts Logbook.xlsx
+++ b/OU Year 3 - 2018/W19 Semester/Senior Project/Projects/Sprints/Sprint 2/Efforts Logbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="3210" windowWidth="23250" windowHeight="13170" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1590" yWindow="3210" windowWidth="23250" windowHeight="13170" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -43,15 +43,6 @@
     <t>Requirements</t>
   </si>
   <si>
-    <t>Class Diagram</t>
-  </si>
-  <si>
-    <t>Design.doc</t>
-  </si>
-  <si>
-    <t>Page 3,4</t>
-  </si>
-  <si>
     <t>Powerpoint</t>
   </si>
   <si>
@@ -215,6 +206,18 @@
   </si>
   <si>
     <t>Page 1 of FURPS, Image file</t>
+  </si>
+  <si>
+    <t>Made 2 Sequence Diagrams, Offered Program for creating them, Helped make Sprint 2 PowerPoint</t>
+  </si>
+  <si>
+    <t>Sequence Diagram</t>
+  </si>
+  <si>
+    <t>Images and PP File zipped with this excel doc</t>
+  </si>
+  <si>
+    <t>small portions of PP, Image Files</t>
   </si>
 </sst>
 </file>
@@ -372,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -408,6 +411,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -420,24 +441,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -449,6 +452,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,7 +728,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -732,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -749,45 +755,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1">
-      <c r="A1" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="A1" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="40.9" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+    </row>
+    <row r="3" spans="1:8" ht="24" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="1:8" ht="24" customHeight="1">
-      <c r="A3" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -803,214 +809,220 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="31.15" customHeight="1">
-      <c r="A4" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="19"/>
+      <c r="A4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="15"/>
       <c r="C4" s="7">
         <v>4</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="19"/>
+      <c r="A6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="15"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="19"/>
+      <c r="A7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="15"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="19"/>
+      <c r="A8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="15"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="19"/>
+      <c r="A9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="15"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="19"/>
+      <c r="A10" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="15"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="19"/>
+      <c r="A11" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="19"/>
+      <c r="A12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="19"/>
+      <c r="A13" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="19"/>
+      <c r="A14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="15"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="19"/>
+      <c r="A15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="15"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="4"/>
@@ -1020,6 +1032,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -1033,11 +1050,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1047,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -1062,11 +1074,11 @@
   <sheetData>
     <row r="1" spans="1:9" ht="34.15" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
@@ -1076,25 +1088,25 @@
       <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:9" ht="40.9" customHeight="1">
-      <c r="A2" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
+      <c r="A2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="22.15" customHeight="1">
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="26" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
@@ -1105,10 +1117,10 @@
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
@@ -1126,18 +1138,18 @@
         <v>5</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="5" customFormat="1" ht="31.15" customHeight="1">
       <c r="A5" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C5" s="11">
         <v>0</v>
@@ -1163,107 +1175,137 @@
     </row>
     <row r="6" spans="1:9" ht="36" customHeight="1">
       <c r="A6" s="10">
+        <v>2</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="29">
+        <v>0</v>
+      </c>
+      <c r="D6" s="29">
+        <v>0</v>
+      </c>
+      <c r="E6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="F6" s="29">
+        <v>0</v>
+      </c>
+      <c r="G6" s="29">
+        <v>0</v>
+      </c>
+      <c r="H6" s="29">
+        <v>0</v>
+      </c>
+      <c r="I6" s="29">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="36" customHeight="1">
       <c r="A7" s="10">
-        <v>2</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
     </row>
     <row r="8" spans="1:9" ht="36" customHeight="1">
       <c r="A8" s="10">
-        <v>3</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
     </row>
     <row r="9" spans="1:9" ht="36" customHeight="1">
       <c r="A9" s="10">
-        <v>4</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="1:9" ht="36" customHeight="1">
       <c r="A10" s="10">
-        <v>5</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
     </row>
     <row r="11" spans="1:9" ht="36" customHeight="1">
       <c r="A11" s="10">
-        <v>6</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
     </row>
     <row r="12" spans="1:9" ht="36" customHeight="1">
       <c r="A12" s="10">
-        <v>7</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:9" ht="36" customHeight="1">
       <c r="A13" s="10">
-        <v>8</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>